<commit_message>
Modificación de la validación
</commit_message>
<xml_diff>
--- a/02/Libro02Paso02.xlsx
+++ b/02/Libro02Paso02.xlsx
@@ -740,7 +740,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -968,8 +968,8 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="El número de votos introducido no es válido" promptTitle="Votos" prompt="Introduzca el número de votos" sqref="B2:F11">
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="El número de unidades introducido no es válido" promptTitle="Unidades" prompt="Introduzca el número de unidades vendidas" sqref="B2:F11">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>